<commit_message>
Update part of the process，异常处理
</commit_message>
<xml_diff>
--- a/API_Test.xlsx
+++ b/API_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="12630" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="currency" sheetId="1" r:id="rId1"/>
@@ -67,13 +67,13 @@
     }</t>
   </si>
   <si>
+    <t>00000002</t>
+  </si>
+  <si>
     <t>Support</t>
   </si>
   <si>
     <t>{"username":"18382133273","password":"123456"}</t>
-  </si>
-  <si>
-    <t>00000002</t>
   </si>
   <si>
     <t>{"userna|me":"18382133273","password":"123456"}</t>
@@ -87,10 +87,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1104,8 +1104,8 @@
   <sheetPr/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1190,7 +1190,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1623,7 +1623,7 @@
   <sheetPr/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1666,7 +1666,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1695,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
@@ -1714,7 +1714,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1757,7 +1757,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
currency interface handle update
</commit_message>
<xml_diff>
--- a/API_Test.xlsx
+++ b/API_Test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t xml:space="preserve">Instruction </t>
   </si>
@@ -56,7 +56,7 @@
     <t>POST</t>
   </si>
   <si>
-    <t>https://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
+    <t>h1ttps://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
   </si>
   <si>
     <t>{"username":"|mobile|","password":"|password|"}</t>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>00000002</t>
+  </si>
+  <si>
+    <t>https://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
   </si>
   <si>
     <t>Support</t>
@@ -87,8 +90,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -123,48 +126,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,46 +141,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,8 +167,79 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,6 +252,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -267,187 +270,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,17 +479,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,17 +512,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,35 +547,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,10 +584,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -593,137 +596,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -753,6 +756,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1105,7 +1111,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1198,8 +1204,8 @@
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
+      <c r="E3" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
@@ -1215,16 +1221,34 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+    <row r="4" ht="165" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10">
@@ -1666,7 +1690,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1692,10 +1716,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
@@ -1723,10 +1747,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>15</v>
@@ -1745,7 +1769,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1754,10 +1778,10 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
common interface add temp
</commit_message>
<xml_diff>
--- a/API_Test.xlsx
+++ b/API_Test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t xml:space="preserve">Instruction </t>
   </si>
@@ -56,7 +56,7 @@
     <t>POST</t>
   </si>
   <si>
-    <t>h1ttps://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
+    <t>https://log1in.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
   </si>
   <si>
     <t>{"username":"|mobile|","password":"|password|"}</t>
@@ -84,16 +84,19 @@
   <si>
     <t>00000003</t>
   </si>
+  <si>
+    <t>00000004</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -117,8 +120,40 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,6 +164,14 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,6 +186,38 @@
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,85 +236,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,9 +250,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -270,6 +273,162 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -282,175 +441,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,26 +482,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,11 +506,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -547,32 +547,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,10 +587,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -596,133 +599,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -757,7 +760,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1174,7 +1177,7 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1204,7 +1207,7 @@
       <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1636,6 +1639,9 @@
       <c r="J36" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://log1in.api.guxiansheng.cn/index.php?c=user&amp;a=login"/>
+  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -1648,7 +1654,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1795,16 +1801,34 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:11">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+    <row r="5" s="1" customFormat="1" ht="66" spans="1:11">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>

</xml_diff>

<commit_message>
Increase the divine budget scripts
</commit_message>
<xml_diff>
--- a/API_Test.xlsx
+++ b/API_Test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t xml:space="preserve">Instruction </t>
   </si>
@@ -56,7 +56,7 @@
     <t>POST</t>
   </si>
   <si>
-    <t>https://log1in.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
+    <t>https://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
   </si>
   <si>
     <t>{"username":"|mobile|","password":"|password|"}</t>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>00000002</t>
-  </si>
-  <si>
-    <t>https://login.api.guxiansheng.cn/index.php?c=user&amp;a=login</t>
   </si>
   <si>
     <t>Support</t>
@@ -118,14 +115,6 @@
       <color theme="1"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -218,6 +207,14 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -602,76 +599,76 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -683,7 +680,7 @@
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -698,10 +695,10 @@
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -710,26 +707,26 @@
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -759,9 +756,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1177,7 +1171,7 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -1208,7 +1202,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>14</v>
@@ -1238,7 +1232,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>14</v>
@@ -1639,9 +1633,6 @@
       <c r="J36" s="6"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://log1in.api.guxiansheng.cn/index.php?c=user&amp;a=login"/>
-  </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -1696,7 +1687,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1722,10 +1713,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>15</v>
@@ -1753,10 +1744,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>15</v>
@@ -1775,7 +1766,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -1784,10 +1775,10 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>15</v>
@@ -1806,7 +1797,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -1815,10 +1806,10 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>15</v>

</xml_diff>